<commit_message>
Vlan beagyazas + ipk
</commit_message>
<xml_diff>
--- a/iptabalazat.xlsx
+++ b/iptabalazat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Portok + IP" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="134">
   <si>
     <t xml:space="preserve">Routerek</t>
   </si>
@@ -357,6 +357,72 @@
   </si>
   <si>
     <t xml:space="preserve">1 – 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hálózatcímtartomány</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Használható IP-k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.43.0/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.43.1 - 172.16.43.126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.42.0/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.42.1 - 172.16.42.126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.41.0/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.41.1 - 172.16.41.126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telep Szeged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.83.0/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.83.1 – 172.16.83.126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.82.0/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.82.1 – 172.16.82.126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.81.0/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.81.1 – 172.16.81.126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.123.0/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.123.1 – 172.16.123.126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.122.0/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.122.1 – 172.16.122.126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.121.0/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.121.1 – 172.16.121.126</t>
   </si>
 </sst>
 </file>
@@ -399,6 +465,7 @@
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -486,7 +553,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -523,10 +590,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -547,6 +610,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -563,8 +630,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -752,7 +827,7 @@
   </sheetPr>
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -1051,7 +1126,7 @@
       <c r="O11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1067,14 +1142,14 @@
       </c>
       <c r="G12" s="1"/>
       <c r="J12" s="8"/>
-      <c r="K12" s="10"/>
+      <c r="K12" s="9"/>
       <c r="L12" s="4"/>
       <c r="M12" s="6"/>
       <c r="N12" s="4"/>
       <c r="O12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9"/>
+      <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
         <v>38</v>
       </c>
@@ -1083,12 +1158,12 @@
         <v>30</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="11"/>
+      <c r="G13" s="10"/>
       <c r="J13" s="8"/>
-      <c r="K13" s="10"/>
+      <c r="K13" s="9"/>
       <c r="L13" s="4"/>
       <c r="M13" s="6"/>
       <c r="N13" s="4"/>
@@ -1164,10 +1239,10 @@
         <v>50</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="J16" s="12" t="s">
+      <c r="J16" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="K16" s="12"/>
+      <c r="K16" s="11"/>
       <c r="L16" s="4" t="s">
         <v>45</v>
       </c>
@@ -1191,10 +1266,10 @@
         <v>53</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="J17" s="12" t="s">
+      <c r="J17" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="K17" s="12"/>
+      <c r="K17" s="11"/>
       <c r="L17" s="4" t="s">
         <v>23</v>
       </c>
@@ -1218,10 +1293,10 @@
         <v>55</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="J18" s="12" t="s">
+      <c r="J18" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="12"/>
+      <c r="K18" s="11"/>
       <c r="L18" s="4" t="s">
         <v>56</v>
       </c>
@@ -1245,10 +1320,10 @@
         <v>58</v>
       </c>
       <c r="G19" s="2"/>
-      <c r="J19" s="13" t="s">
+      <c r="J19" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="K19" s="13"/>
+      <c r="K19" s="12"/>
       <c r="L19" s="4" t="s">
         <v>60</v>
       </c>
@@ -1273,8 +1348,8 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="6"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="14"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="13"/>
       <c r="L20" s="4"/>
       <c r="M20" s="6"/>
       <c r="N20" s="4"/>
@@ -1282,10 +1357,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="11"/>
+      <c r="C21" s="10"/>
       <c r="D21" s="1" t="s">
         <v>18</v>
       </c>
@@ -1294,8 +1369,8 @@
         <v>63</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="14"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="13"/>
       <c r="L21" s="4"/>
       <c r="M21" s="6"/>
       <c r="N21" s="4"/>
@@ -1303,10 +1378,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="11"/>
+      <c r="C22" s="10"/>
       <c r="D22" s="1" t="s">
         <v>11</v>
       </c>
@@ -1315,10 +1390,10 @@
         <v>64</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="J22" s="13" t="s">
+      <c r="J22" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="K22" s="13"/>
+      <c r="K22" s="12"/>
       <c r="L22" s="4" t="s">
         <v>65</v>
       </c>
@@ -1394,7 +1469,7 @@
       <c r="O25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9"/>
+      <c r="A26" s="14"/>
       <c r="B26" s="1" t="s">
         <v>70</v>
       </c>
@@ -1427,14 +1502,14 @@
         <v>74</v>
       </c>
       <c r="G27" s="1"/>
-      <c r="J27" s="11" t="s">
+      <c r="J27" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
@@ -1876,13 +1951,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.32"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
@@ -1951,6 +2030,158 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19"/>
       <c r="B6" s="19"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>133</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>